<commit_message>
Add updated Student 4 docs
</commit_message>
<xml_diff>
--- a/reports/Student #4/z-test.xlsx
+++ b/reports/Student #4/z-test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\UNI\PSG\Workspace-25\Projects\DP2-C01-31\reports\Student #4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D00D80F-D32B-4D8C-AEB6-D94E5DE8E3F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5869F5B5-BE4C-4E21-8F10-5B551D474FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10350" yWindow="0" windowWidth="18555" windowHeight="15585" xr2:uid="{E8722665-0605-4E63-8DF6-EF025A332097}"/>
+    <workbookView xWindow="9885" yWindow="2070" windowWidth="16245" windowHeight="11295" xr2:uid="{E8722665-0605-4E63-8DF6-EF025A332097}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Before</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Valor crítico de z (dos colas)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -135,11 +138,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF6A771-66EA-4793-9618-CABB19F6AF4E}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,100 +497,100 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>9.8321140649221501</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>8.6548709299451012</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>159.59111799999999</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>131.26536300000001</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>514</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>514</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>0</v>
       </c>
-      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>1.5649784202349371</v>
       </c>
-      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <v>5.8793984661719478E-2</v>
       </c>
-      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>1.6448536269514715</v>
       </c>
-      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>0.117587969323439</v>
       </c>
-      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>1.9599639845400536</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>